<commit_message>
Add comparison for each MSE to best MSE within each group (e.g. heavy vs. light)
</commit_message>
<xml_diff>
--- a/jim/model_testing_assignment_jim.xlsx
+++ b/jim/model_testing_assignment_jim.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>users</t>
   </si>
@@ -30,141 +30,29 @@
     <t>Cross-validated Mean-Squared Error</t>
   </si>
   <si>
-    <t>If you want to use CV code I wrote you can follow:</t>
-  </si>
-  <si>
     <t>heavy</t>
   </si>
   <si>
     <t>level-level</t>
   </si>
   <si>
-    <t>jim</t>
-  </si>
-  <si>
-    <t>Copy and paste 06_cross_val_model_selection.R into your named folder</t>
-  </si>
-  <si>
     <t>Semi-log</t>
   </si>
   <si>
-    <t>julian</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ensure you have the data (named as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>InstantCoffee.csv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>) inside the data folder of the project directory</t>
-    </r>
-  </si>
-  <si>
     <t>log-log</t>
   </si>
   <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>Open the R studio project in the root directory of the project folder (this sets your working directory)</t>
-  </si>
-  <si>
     <t>light</t>
   </si>
   <si>
-    <t>tina</t>
-  </si>
-  <si>
-    <r>
-      <t>Run line 3 in the file (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>source(“./r/analysis.R”)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">), this should create 3 objects, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>coffee_clean; heavy; light</t>
-    </r>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>Change line 7 to be the users you want to model (i.e. either heavy or light)</t>
-  </si>
-  <si>
-    <t>jessica</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">At line 50, change the functional form of the model to be that you're working on: ie log-transform with </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>log()</t>
-    </r>
-  </si>
-  <si>
-    <t>Run the script from Step 1 onwards, it should compute a single average MSE that we can use to assess model quality.</t>
-  </si>
-  <si>
-    <t>Any questions let me know, I'll be online most/all of the day</t>
+    <t>vs best for group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -173,20 +61,31 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -198,17 +97,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,25 +391,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625"/>
     <col min="2" max="2" width="10.5703125"/>
-    <col min="3" max="3" width="30.7109375"/>
-    <col min="4" max="4" width="6.85546875"/>
-    <col min="5" max="5" width="8.5703125"/>
-    <col min="6" max="6" width="13.28515625"/>
-    <col min="7" max="7" width="123.5703125" customWidth="1"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625"/>
+    <col min="7" max="1024" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,141 +417,98 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>193.10176000000001</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2">
+        <f>1-C2/IF(A2="heavy",MIN($C$2:$C$4), MIN($C$5:$C$7))</f>
+        <v>-1.2061928191532623E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>190.80034000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D7" si="0">1-C3/IF(A3="heavy",MIN($C$2:$C$4), MIN($C$5:$C$7))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>190.80034000000001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>230.78298000000001</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20955224712911935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>70.279750000000007</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="C5">
-        <v>70.279750000000007</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
       <c r="C6">
         <v>79.490939999999995</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13106463810699376</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>75.414519999999996</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>22</v>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.3061870595726219E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>